<commit_message>
Added activities, models and variables.
</commit_message>
<xml_diff>
--- a/GenericScenarioEvaluation/Reviewed Scenarios/ST/Use of textile dyes.xlsx
+++ b/GenericScenarioEvaluation/Reviewed Scenarios/ST/Use of textile dyes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/barrett_williamm_epa_gov/Documents/Repos/GenericScenarioEvaluation/GenericScenarioEvaluation/Reviewed Scenarios/ST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="585" documentId="8_{B8A40B9A-7899-4EDF-9FB8-C7E519DE68A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{59695946-EA10-479B-95D3-A534540E25D4}"/>
+  <xr:revisionPtr revIDLastSave="586" documentId="8_{B8A40B9A-7899-4EDF-9FB8-C7E519DE68A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7C601F86-7711-4F97-8747-E83A0520FB49}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AEE7231D-D110-46BA-BB08-35ECB9C6F51B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AEE7231D-D110-46BA-BB08-35ECB9C6F51B}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -717,10 +717,6 @@
     <t>Dermal exposure is expected for both automated and manual unloading/transferring activities.</t>
   </si>
   <si>
-    <t>EPA/OPPT 2-Hand Dermal Contact with
-Liquid Model; EPA/OPPT Direct 2-Hand Dermal Contact with Solids Model.</t>
-  </si>
-  <si>
     <t>Inhalation exposure from dust particulates during the cleaning of solid powders from transport containers.</t>
   </si>
   <si>
@@ -1108,6 +1104,9 @@
   </si>
   <si>
     <t>Kg/site-day</t>
+  </si>
+  <si>
+    <t>EPA/OPPT 2-Hand Dermal Contact with Liquid Model; EPA/OPPT Direct 2-Hand Dermal Contact with Solids Model.</t>
   </si>
 </sst>
 </file>
@@ -2168,7 +2167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8A8DA8E-F055-4EAE-98B3-B13E29507A62}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -2198,7 +2197,7 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E2" s="5"/>
     </row>
@@ -2397,8 +2396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE2C11F-6A25-4CA6-B493-2A0028270B50}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2453,7 +2452,7 @@
         <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>34</v>
@@ -2525,7 +2524,7 @@
         <v>205</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -2551,7 +2550,7 @@
         <v>208</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
@@ -2574,7 +2573,7 @@
         <v>62</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -2615,7 +2614,7 @@
         <v>194</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2633,7 +2632,7 @@
         <v>194</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>216</v>
+        <v>339</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2641,7 +2640,7 @@
         <v>213</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
@@ -2650,13 +2649,13 @@
         <v>194</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
@@ -2668,15 +2667,15 @@
         <v>194</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -2688,7 +2687,7 @@
         <v>194</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2816,20 +2815,20 @@
         <v>174</v>
       </c>
       <c r="E2" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>225</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>204</v>
@@ -2850,7 +2849,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="2"/>
       <c r="H3" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I3" s="7">
         <v>0.5</v>
@@ -2860,14 +2859,14 @@
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N3" s="7"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
@@ -2877,20 +2876,20 @@
         <v>174</v>
       </c>
       <c r="E4" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>225</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
@@ -2907,11 +2906,11 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
@@ -2928,20 +2927,20 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I6" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P6" s="7"/>
     </row>
@@ -2953,11 +2952,11 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
@@ -2984,7 +2983,7 @@
     </row>
     <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2992,20 +2991,20 @@
         <v>174</v>
       </c>
       <c r="E9" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>225</v>
-      </c>
       <c r="G9" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
@@ -3024,11 +3023,11 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
@@ -3045,18 +3044,18 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
       <c r="O11" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P11" s="7"/>
     </row>
@@ -3068,11 +3067,11 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -3086,24 +3085,24 @@
         <v>205</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>225</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
@@ -3122,11 +3121,11 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
@@ -3143,11 +3142,11 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
@@ -3164,11 +3163,11 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
@@ -3185,11 +3184,11 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
@@ -3206,11 +3205,11 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
@@ -3227,11 +3226,11 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
@@ -3248,7 +3247,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="I20" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="7"/>
@@ -3266,11 +3265,11 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
@@ -3289,11 +3288,11 @@
       <c r="F22" s="17"/>
       <c r="G22" s="7"/>
       <c r="H22" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
@@ -3309,18 +3308,18 @@
       <c r="F23" s="17"/>
       <c r="G23" s="7"/>
       <c r="H23" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -3331,19 +3330,19 @@
         <v>175</v>
       </c>
       <c r="E24" t="s">
+        <v>223</v>
+      </c>
+      <c r="F24" t="s">
         <v>224</v>
       </c>
-      <c r="F24" t="s">
-        <v>225</v>
-      </c>
       <c r="G24" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N24" t="s">
         <v>186</v>
@@ -3351,18 +3350,18 @@
     </row>
     <row r="25" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="H25" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="H26" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -3376,19 +3375,19 @@
         <v>175</v>
       </c>
       <c r="E27" t="s">
+        <v>223</v>
+      </c>
+      <c r="F27" t="s">
         <v>224</v>
       </c>
-      <c r="F27" t="s">
-        <v>225</v>
-      </c>
       <c r="G27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N27" t="s">
         <v>186</v>
@@ -3396,29 +3395,29 @@
     </row>
     <row r="28" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="H28" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="H29" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="O29" t="s">
         <v>270</v>
-      </c>
-      <c r="O29" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="C31" t="s">
         <v>47</v>
@@ -3427,19 +3426,19 @@
         <v>174</v>
       </c>
       <c r="E31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F31" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G31" t="s">
         <v>178</v>
       </c>
       <c r="H31" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="J31" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>276</v>
       </c>
       <c r="N31" t="s">
         <v>186</v>
@@ -3447,60 +3446,60 @@
     </row>
     <row r="32" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="H32" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H33" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="J33" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="J33" s="7" t="s">
-        <v>279</v>
-      </c>
       <c r="O33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="H35" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="J35" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D36" t="s">
         <v>174</v>
       </c>
       <c r="E36" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G36" t="s">
         <v>178</v>
       </c>
       <c r="H36" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="J36" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>276</v>
       </c>
       <c r="N36" t="s">
         <v>186</v>
@@ -3511,37 +3510,37 @@
         <v>47</v>
       </c>
       <c r="H37" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="H38" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="H39" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="J39" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="J39" s="2" t="s">
-        <v>291</v>
-      </c>
       <c r="O39" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C40" t="s">
         <v>172</v>
@@ -3550,16 +3549,16 @@
         <v>175</v>
       </c>
       <c r="E40" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F40" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H40" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="J40" s="2" t="s">
         <v>293</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>294</v>
       </c>
       <c r="N40" t="s">
         <v>186</v>
@@ -3567,57 +3566,57 @@
     </row>
     <row r="41" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="H41" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="I41" t="s">
+        <v>296</v>
+      </c>
+      <c r="J41" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="I41" t="s">
+      <c r="O41" t="s">
         <v>297</v>
-      </c>
-      <c r="J41" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="O41" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="H42" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I42">
         <v>1070</v>
       </c>
       <c r="J42" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="O42" t="s">
         <v>300</v>
-      </c>
-      <c r="O42" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H43" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I43">
         <v>1</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="H44" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C45" t="s">
         <v>172</v>
@@ -3626,16 +3625,16 @@
         <v>174</v>
       </c>
       <c r="E45" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F45" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H45" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="J45" s="2" t="s">
         <v>293</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>294</v>
       </c>
       <c r="N45" t="s">
         <v>186</v>
@@ -3643,35 +3642,35 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H46" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I46">
         <v>1</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="H47" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H48" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="J48" s="2" t="s">
         <v>308</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>309</v>
       </c>
       <c r="N48" t="s">
         <v>186</v>
@@ -3679,29 +3678,29 @@
     </row>
     <row r="49" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="H49" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="H50" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I50" t="s">
+        <v>312</v>
+      </c>
+      <c r="J50" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>317</v>
       </c>
       <c r="C51" t="s">
         <v>47</v>
@@ -3710,16 +3709,16 @@
         <v>174</v>
       </c>
       <c r="E51" t="s">
+        <v>273</v>
+      </c>
+      <c r="F51" t="s">
+        <v>224</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="F51" t="s">
-        <v>225</v>
-      </c>
-      <c r="H51" s="1" t="s">
+      <c r="J51" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>276</v>
       </c>
       <c r="N51" t="s">
         <v>186</v>
@@ -3727,51 +3726,51 @@
     </row>
     <row r="52" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="H52" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I52">
         <v>15</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H53" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I53">
         <v>1.25</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="O53" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H54" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I54">
         <v>8</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="H55" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="J55" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C56" t="s">
         <v>47</v>
@@ -3780,16 +3779,16 @@
         <v>174</v>
       </c>
       <c r="E56" t="s">
+        <v>273</v>
+      </c>
+      <c r="F56" t="s">
+        <v>224</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="F56" t="s">
-        <v>225</v>
-      </c>
-      <c r="H56" s="1" t="s">
+      <c r="J56" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>276</v>
       </c>
       <c r="N56" t="s">
         <v>186</v>
@@ -3797,37 +3796,37 @@
     </row>
     <row r="57" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="H57" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="H58" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="J58" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="H59" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I59" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C60" t="s">
         <v>172</v>
@@ -3836,16 +3835,16 @@
         <v>175</v>
       </c>
       <c r="E60" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H60" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="J60" s="2" t="s">
         <v>293</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>294</v>
       </c>
       <c r="N60" t="s">
         <v>186</v>
@@ -3853,49 +3852,49 @@
     </row>
     <row r="61" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="H61" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="I61" t="s">
+        <v>324</v>
+      </c>
+      <c r="J61" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="I61" t="s">
-        <v>325</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>296</v>
-      </c>
       <c r="O61" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H62" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I62" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O62" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H63" t="s">
+        <v>304</v>
+      </c>
+      <c r="I63" t="s">
+        <v>326</v>
+      </c>
+      <c r="J63" s="7" t="s">
         <v>305</v>
-      </c>
-      <c r="I63" t="s">
-        <v>327</v>
-      </c>
-      <c r="J63" s="7" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="H64" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="J64" s="2" t="s">
         <v>329</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -4494,45 +4493,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
-    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
-    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2021-03-04T14:13:47+00:00</Document_x0020_Creation_x0020_Date>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j747ac98061d40f0aa7bd47e1db5675d>
-    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Creator>
-    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </EPA_x0020_Contributor>
-    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F11D2A2FBBEED40A750386529AFE883" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a7fcd2fa88e0328b3b0dd9ef335fe48c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="241d41d8-5778-4e30-b44e-dee891c66b79" xmlns:ns6="af43f131-d884-42a1-ba66-3c1404ec48fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a2a87f8101accce6a0d0ea40fd00900" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4965,42 +4939,62 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2021-03-04T14:13:47+00:00</Document_x0020_Creation_x0020_Date>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F27FAEFF-543C-4C30-A571-905BD321BEF9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E9A4B38-4D52-46C0-9803-4EB30CC27F1C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="241d41d8-5778-4e30-b44e-dee891c66b79"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="af43f131-d884-42a1-ba66-3c1404ec48fc"/>
-    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3227138-1B8A-4733-BA76-D224862EAA4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B3BCB7C-2988-4E98-8C64-AB141F529DE5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5023,18 +5017,23 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3227138-1B8A-4733-BA76-D224862EAA4A}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F27FAEFF-543C-4C30-A571-905BD321BEF9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E9A4B38-4D52-46C0-9803-4EB30CC27F1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="241d41d8-5778-4e30-b44e-dee891c66b79"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="af43f131-d884-42a1-ba66-3c1404ec48fc"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>